<commit_message>
fix up tests and implementation
</commit_message>
<xml_diff>
--- a/data_capture/static/data_capture/r10_example.xlsx
+++ b/data_capture/static/data_capture/r10_example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="13900" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14620" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <definedName name="UnitOther">#REF!</definedName>
     <definedName name="Unittrans">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="102">
   <si>
     <r>
       <t>Note: If Proposing ODCs With A Markup</t>
@@ -838,9 +838,6 @@
     <t>Customer Site</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>Disposal Services</t>
   </si>
   <si>
@@ -860,9 +857,6 @@
   </si>
   <si>
     <t>Both</t>
-  </si>
-  <si>
-    <t>Professional Certification</t>
   </si>
   <si>
     <t>Consultant II</t>
@@ -945,6 +939,9 @@
   </si>
   <si>
     <t>SIN(s) Proposed</t>
+  </si>
+  <si>
+    <t>Bachelors</t>
   </si>
 </sst>
 </file>
@@ -954,9 +951,16 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1203,125 +1207,125 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
@@ -1362,145 +1366,145 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="17" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="17" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="10" fontId="18" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="44" fontId="19" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="10" fontId="17" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="17" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="17" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="17" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="10" fontId="18" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="18" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="18" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="44" fontId="17" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="18" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="17" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="18" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="17" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="18" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="17" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="18" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="21" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="22" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="23" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="23" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="23" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="22" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="44" fontId="22" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="22" fillId="6" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="21" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="21" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="21" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="22" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2383,7 +2387,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -2402,7 +2406,7 @@
   <dimension ref="A1:Q58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScale="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2429,109 +2433,105 @@
   <sheetData>
     <row r="1" spans="1:17" s="83" customFormat="1" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="90" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B1" s="90" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C1" s="90" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D1" s="92" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E1" s="92" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F1" s="92" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G1" s="91" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H1" s="90" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I1" s="90" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J1" s="89" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K1" s="87" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="L1" s="88" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M1" s="87" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="N1" s="87" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O1" s="86" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="P1" s="85" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="Q1" s="84" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="75" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="78" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B2" s="82" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C2" s="81" t="s">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="D2" s="80">
         <v>2</v>
       </c>
       <c r="E2" s="79" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F2" s="79" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G2" s="73">
         <v>100</v>
       </c>
       <c r="H2" s="78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I2" s="77" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J2" s="69">
-        <f>IFERROR(1-(K2/G2),"")</f>
         <v>5.0000000000000044E-2</v>
       </c>
       <c r="K2" s="73">
         <v>95</v>
       </c>
       <c r="L2" s="69">
-        <f>IFERROR(1-(M2/G2),"")</f>
         <v>9.9999999999999978E-2</v>
       </c>
       <c r="M2" s="73">
         <v>90</v>
       </c>
       <c r="N2" s="67">
-        <f>M2/0.9925</f>
-        <v>90.680100755667496</v>
+        <v>90.68</v>
       </c>
       <c r="O2" s="66">
-        <f>IFERROR((K2-M2)/K2,"")</f>
-        <v>5.2631578947368418E-2</v>
+        <v>5.2600000000000001E-2</v>
       </c>
       <c r="P2" s="76" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q2" s="76">
         <v>1</v>
@@ -2539,14 +2539,12 @@
     </row>
     <row r="3" spans="1:17" s="52" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="72" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="71" t="s">
-        <v>76</v>
-      </c>
-      <c r="C3" s="71" t="s">
         <v>75</v>
       </c>
+      <c r="C3" s="71"/>
       <c r="D3" s="74">
         <v>0</v>
       </c>
@@ -2569,22 +2567,18 @@
         <v>0</v>
       </c>
       <c r="K3" s="68">
-        <f>G3-SUM(G3*J3)</f>
         <v>100</v>
       </c>
       <c r="L3" s="69">
-        <f>IFERROR(1-(M3/G3),"")</f>
         <v>1</v>
       </c>
       <c r="M3" s="68">
         <v>0</v>
       </c>
       <c r="N3" s="67">
-        <f>M3/0.9925</f>
         <v>0</v>
       </c>
       <c r="O3" s="66">
-        <f>IFERROR((K3-M3)/K3,"")</f>
         <v>1</v>
       </c>
       <c r="P3" s="65" t="s">
@@ -2605,25 +2599,25 @@
       <c r="H4" s="60"/>
       <c r="I4" s="59"/>
       <c r="J4" s="58" t="str">
-        <f>IFERROR(1-(K4/G4),"")</f>
+        <f t="shared" ref="J4:J35" si="0">IFERROR(1-(K4/G4),"")</f>
         <v/>
       </c>
       <c r="K4" s="57">
         <v>0</v>
       </c>
       <c r="L4" s="58" t="str">
-        <f>IFERROR(1-(M4/G4),"")</f>
+        <f t="shared" ref="L2:L33" si="1">IFERROR(1-(M4/G4),"")</f>
         <v/>
       </c>
       <c r="M4" s="57">
         <v>0</v>
       </c>
       <c r="N4" s="56">
-        <f>M4/0.9925</f>
+        <f t="shared" ref="N2:N33" si="2">M4/0.9925</f>
         <v>0</v>
       </c>
       <c r="O4" s="55" t="str">
-        <f>IFERROR((K4-M4)/K4,"")</f>
+        <f t="shared" ref="O2:O33" si="3">IFERROR((K4-M4)/K4,"")</f>
         <v/>
       </c>
       <c r="P4" s="54"/>
@@ -2642,25 +2636,25 @@
       <c r="H5" s="60"/>
       <c r="I5" s="59"/>
       <c r="J5" s="58" t="str">
-        <f>IFERROR(1-(K5/G5),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K5" s="57">
         <v>0</v>
       </c>
       <c r="L5" s="58" t="str">
-        <f>IFERROR(1-(M5/G5),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M5" s="57">
         <v>0</v>
       </c>
       <c r="N5" s="56">
-        <f>M5/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O5" s="55" t="str">
-        <f>IFERROR((K5-M5)/K5,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P5" s="54"/>
@@ -2677,25 +2671,25 @@
       <c r="H6" s="60"/>
       <c r="I6" s="59"/>
       <c r="J6" s="58" t="str">
-        <f>IFERROR(1-(K6/G6),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K6" s="57">
         <v>0</v>
       </c>
       <c r="L6" s="58" t="str">
-        <f>IFERROR(1-(M6/G6),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M6" s="57">
         <v>0</v>
       </c>
       <c r="N6" s="56">
-        <f>M6/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O6" s="55" t="str">
-        <f>IFERROR((K6-M6)/K6,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P6" s="54"/>
@@ -2712,25 +2706,25 @@
       <c r="H7" s="60"/>
       <c r="I7" s="59"/>
       <c r="J7" s="58" t="str">
-        <f>IFERROR(1-(K7/G7),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K7" s="57">
         <v>0</v>
       </c>
       <c r="L7" s="58" t="str">
-        <f>IFERROR(1-(M7/G7),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M7" s="57">
         <v>0</v>
       </c>
       <c r="N7" s="56">
-        <f>M7/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O7" s="55" t="str">
-        <f>IFERROR((K7-M7)/K7,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P7" s="54"/>
@@ -2747,25 +2741,25 @@
       <c r="H8" s="60"/>
       <c r="I8" s="59"/>
       <c r="J8" s="58" t="str">
-        <f>IFERROR(1-(K8/G8),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K8" s="57">
         <v>0</v>
       </c>
       <c r="L8" s="58" t="str">
-        <f>IFERROR(1-(M8/G8),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M8" s="57">
         <v>0</v>
       </c>
       <c r="N8" s="56">
-        <f>M8/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O8" s="55" t="str">
-        <f>IFERROR((K8-M8)/K8,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P8" s="54"/>
@@ -2782,25 +2776,25 @@
       <c r="H9" s="60"/>
       <c r="I9" s="59"/>
       <c r="J9" s="58" t="str">
-        <f>IFERROR(1-(K9/G9),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K9" s="57">
         <v>0</v>
       </c>
       <c r="L9" s="58" t="str">
-        <f>IFERROR(1-(M9/G9),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M9" s="57">
         <v>0</v>
       </c>
       <c r="N9" s="56">
-        <f>M9/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O9" s="55" t="str">
-        <f>IFERROR((K9-M9)/K9,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P9" s="54"/>
@@ -2817,25 +2811,25 @@
       <c r="H10" s="60"/>
       <c r="I10" s="59"/>
       <c r="J10" s="58" t="str">
-        <f>IFERROR(1-(K10/G10),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K10" s="57">
         <v>0</v>
       </c>
       <c r="L10" s="58" t="str">
-        <f>IFERROR(1-(M10/G10),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M10" s="57">
         <v>0</v>
       </c>
       <c r="N10" s="56">
-        <f>M10/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O10" s="55" t="str">
-        <f>IFERROR((K10-M10)/K10,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P10" s="54"/>
@@ -2852,25 +2846,25 @@
       <c r="H11" s="60"/>
       <c r="I11" s="59"/>
       <c r="J11" s="58" t="str">
-        <f>IFERROR(1-(K11/G11),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K11" s="57">
         <v>0</v>
       </c>
       <c r="L11" s="58" t="str">
-        <f>IFERROR(1-(M11/G11),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M11" s="57">
         <v>0</v>
       </c>
       <c r="N11" s="56">
-        <f>M11/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O11" s="55" t="str">
-        <f>IFERROR((K11-M11)/K11,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P11" s="54"/>
@@ -2887,25 +2881,25 @@
       <c r="H12" s="60"/>
       <c r="I12" s="59"/>
       <c r="J12" s="58" t="str">
-        <f>IFERROR(1-(K12/G12),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K12" s="57">
         <v>0</v>
       </c>
       <c r="L12" s="58" t="str">
-        <f>IFERROR(1-(M12/G12),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M12" s="57">
         <v>0</v>
       </c>
       <c r="N12" s="56">
-        <f>M12/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O12" s="55" t="str">
-        <f>IFERROR((K12-M12)/K12,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P12" s="54"/>
@@ -2922,25 +2916,25 @@
       <c r="H13" s="60"/>
       <c r="I13" s="59"/>
       <c r="J13" s="58" t="str">
-        <f>IFERROR(1-(K13/G13),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K13" s="57">
         <v>0</v>
       </c>
       <c r="L13" s="58" t="str">
-        <f>IFERROR(1-(M13/G13),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M13" s="57">
         <v>0</v>
       </c>
       <c r="N13" s="56">
-        <f>M13/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O13" s="55" t="str">
-        <f>IFERROR((K13-M13)/K13,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P13" s="54"/>
@@ -2957,25 +2951,25 @@
       <c r="H14" s="60"/>
       <c r="I14" s="59"/>
       <c r="J14" s="58" t="str">
-        <f>IFERROR(1-(K14/G14),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K14" s="57">
         <v>0</v>
       </c>
       <c r="L14" s="58" t="str">
-        <f>IFERROR(1-(M14/G14),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M14" s="57">
         <v>0</v>
       </c>
       <c r="N14" s="56">
-        <f>M14/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O14" s="55" t="str">
-        <f>IFERROR((K14-M14)/K14,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P14" s="54"/>
@@ -2992,25 +2986,25 @@
       <c r="H15" s="60"/>
       <c r="I15" s="59"/>
       <c r="J15" s="58" t="str">
-        <f>IFERROR(1-(K15/G15),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K15" s="57">
         <v>0</v>
       </c>
       <c r="L15" s="58" t="str">
-        <f>IFERROR(1-(M15/G15),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M15" s="57">
         <v>0</v>
       </c>
       <c r="N15" s="56">
-        <f>M15/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O15" s="55" t="str">
-        <f>IFERROR((K15-M15)/K15,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P15" s="54"/>
@@ -3027,25 +3021,25 @@
       <c r="H16" s="60"/>
       <c r="I16" s="59"/>
       <c r="J16" s="58" t="str">
-        <f>IFERROR(1-(K16/G16),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K16" s="57">
         <v>0</v>
       </c>
       <c r="L16" s="58" t="str">
-        <f>IFERROR(1-(M16/G16),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M16" s="57">
         <v>0</v>
       </c>
       <c r="N16" s="56">
-        <f>M16/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O16" s="55" t="str">
-        <f>IFERROR((K16-M16)/K16,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P16" s="54"/>
@@ -3064,25 +3058,25 @@
       <c r="H17" s="60"/>
       <c r="I17" s="59"/>
       <c r="J17" s="58" t="str">
-        <f>IFERROR(1-(K17/G17),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K17" s="57">
         <v>0</v>
       </c>
       <c r="L17" s="58" t="str">
-        <f>IFERROR(1-(M17/G17),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M17" s="57">
         <v>0</v>
       </c>
       <c r="N17" s="56">
-        <f>M17/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O17" s="55" t="str">
-        <f>IFERROR((K17-M17)/K17,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P17" s="54"/>
@@ -3099,25 +3093,25 @@
       <c r="H18" s="60"/>
       <c r="I18" s="59"/>
       <c r="J18" s="58" t="str">
-        <f>IFERROR(1-(K18/G18),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K18" s="57">
         <v>0</v>
       </c>
       <c r="L18" s="58" t="str">
-        <f>IFERROR(1-(M18/G18),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M18" s="57">
         <v>0</v>
       </c>
       <c r="N18" s="56">
-        <f>M18/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O18" s="55" t="str">
-        <f>IFERROR((K18-M18)/K18,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P18" s="54"/>
@@ -3134,25 +3128,25 @@
       <c r="H19" s="60"/>
       <c r="I19" s="59"/>
       <c r="J19" s="58" t="str">
-        <f>IFERROR(1-(K19/G19),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K19" s="57">
         <v>0</v>
       </c>
       <c r="L19" s="58" t="str">
-        <f>IFERROR(1-(M19/G19),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M19" s="57">
         <v>0</v>
       </c>
       <c r="N19" s="56">
-        <f>M19/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O19" s="55" t="str">
-        <f>IFERROR((K19-M19)/K19,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P19" s="54"/>
@@ -3169,25 +3163,25 @@
       <c r="H20" s="60"/>
       <c r="I20" s="59"/>
       <c r="J20" s="58" t="str">
-        <f>IFERROR(1-(K20/G20),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K20" s="57">
         <v>0</v>
       </c>
       <c r="L20" s="58" t="str">
-        <f>IFERROR(1-(M20/G20),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M20" s="57">
         <v>0</v>
       </c>
       <c r="N20" s="56">
-        <f>M20/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O20" s="55" t="str">
-        <f>IFERROR((K20-M20)/K20,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P20" s="54"/>
@@ -3204,25 +3198,25 @@
       <c r="H21" s="60"/>
       <c r="I21" s="59"/>
       <c r="J21" s="58" t="str">
-        <f>IFERROR(1-(K21/G21),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K21" s="57">
         <v>0</v>
       </c>
       <c r="L21" s="58" t="str">
-        <f>IFERROR(1-(M21/G21),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M21" s="57">
         <v>0</v>
       </c>
       <c r="N21" s="56">
-        <f>M21/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O21" s="55" t="str">
-        <f>IFERROR((K21-M21)/K21,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P21" s="54"/>
@@ -3239,25 +3233,25 @@
       <c r="H22" s="60"/>
       <c r="I22" s="59"/>
       <c r="J22" s="58" t="str">
-        <f>IFERROR(1-(K22/G22),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K22" s="57">
         <v>0</v>
       </c>
       <c r="L22" s="58" t="str">
-        <f>IFERROR(1-(M22/G22),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M22" s="57">
         <v>0</v>
       </c>
       <c r="N22" s="56">
-        <f>M22/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O22" s="55" t="str">
-        <f>IFERROR((K22-M22)/K22,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P22" s="54"/>
@@ -3274,25 +3268,25 @@
       <c r="H23" s="60"/>
       <c r="I23" s="59"/>
       <c r="J23" s="58" t="str">
-        <f>IFERROR(1-(K23/G23),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K23" s="57">
         <v>0</v>
       </c>
       <c r="L23" s="58" t="str">
-        <f>IFERROR(1-(M23/G23),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M23" s="57">
         <v>0</v>
       </c>
       <c r="N23" s="56">
-        <f>M23/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O23" s="55" t="str">
-        <f>IFERROR((K23-M23)/K23,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P23" s="54"/>
@@ -3309,25 +3303,25 @@
       <c r="H24" s="60"/>
       <c r="I24" s="59"/>
       <c r="J24" s="58" t="str">
-        <f>IFERROR(1-(K24/G24),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K24" s="57">
         <v>0</v>
       </c>
       <c r="L24" s="58" t="str">
-        <f>IFERROR(1-(M24/G24),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M24" s="57">
         <v>0</v>
       </c>
       <c r="N24" s="56">
-        <f>M24/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O24" s="55" t="str">
-        <f>IFERROR((K24-M24)/K24,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P24" s="54"/>
@@ -3344,25 +3338,25 @@
       <c r="H25" s="60"/>
       <c r="I25" s="59"/>
       <c r="J25" s="58" t="str">
-        <f>IFERROR(1-(K25/G25),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K25" s="57">
         <v>0</v>
       </c>
       <c r="L25" s="58" t="str">
-        <f>IFERROR(1-(M25/G25),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M25" s="57">
         <v>0</v>
       </c>
       <c r="N25" s="56">
-        <f>M25/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O25" s="55" t="str">
-        <f>IFERROR((K25-M25)/K25,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P25" s="54"/>
@@ -3379,25 +3373,25 @@
       <c r="H26" s="60"/>
       <c r="I26" s="59"/>
       <c r="J26" s="58" t="str">
-        <f>IFERROR(1-(K26/G26),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K26" s="57">
         <v>0</v>
       </c>
       <c r="L26" s="58" t="str">
-        <f>IFERROR(1-(M26/G26),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M26" s="57">
         <v>0</v>
       </c>
       <c r="N26" s="56">
-        <f>M26/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O26" s="55" t="str">
-        <f>IFERROR((K26-M26)/K26,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P26" s="54"/>
@@ -3414,25 +3408,25 @@
       <c r="H27" s="60"/>
       <c r="I27" s="59"/>
       <c r="J27" s="58" t="str">
-        <f>IFERROR(1-(K27/G27),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K27" s="57">
         <v>0</v>
       </c>
       <c r="L27" s="58" t="str">
-        <f>IFERROR(1-(M27/G27),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M27" s="57">
         <v>0</v>
       </c>
       <c r="N27" s="56">
-        <f>M27/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O27" s="55" t="str">
-        <f>IFERROR((K27-M27)/K27,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P27" s="54"/>
@@ -3449,25 +3443,25 @@
       <c r="H28" s="60"/>
       <c r="I28" s="59"/>
       <c r="J28" s="58" t="str">
-        <f>IFERROR(1-(K28/G28),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K28" s="57">
         <v>0</v>
       </c>
       <c r="L28" s="58" t="str">
-        <f>IFERROR(1-(M28/G28),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M28" s="57">
         <v>0</v>
       </c>
       <c r="N28" s="56">
-        <f>M28/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O28" s="55" t="str">
-        <f>IFERROR((K28-M28)/K28,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P28" s="54"/>
@@ -3484,25 +3478,25 @@
       <c r="H29" s="60"/>
       <c r="I29" s="59"/>
       <c r="J29" s="58" t="str">
-        <f>IFERROR(1-(K29/G29),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K29" s="57">
         <v>0</v>
       </c>
       <c r="L29" s="58" t="str">
-        <f>IFERROR(1-(M29/G29),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M29" s="57">
         <v>0</v>
       </c>
       <c r="N29" s="56">
-        <f>M29/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O29" s="55" t="str">
-        <f>IFERROR((K29-M29)/K29,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P29" s="54"/>
@@ -3519,25 +3513,25 @@
       <c r="H30" s="60"/>
       <c r="I30" s="59"/>
       <c r="J30" s="58" t="str">
-        <f>IFERROR(1-(K30/G30),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K30" s="57">
         <v>0</v>
       </c>
       <c r="L30" s="58" t="str">
-        <f>IFERROR(1-(M30/G30),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M30" s="57">
         <v>0</v>
       </c>
       <c r="N30" s="56">
-        <f>M30/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O30" s="55" t="str">
-        <f>IFERROR((K30-M30)/K30,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P30" s="54"/>
@@ -3554,25 +3548,25 @@
       <c r="H31" s="60"/>
       <c r="I31" s="59"/>
       <c r="J31" s="58" t="str">
-        <f>IFERROR(1-(K31/G31),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K31" s="57">
         <v>0</v>
       </c>
       <c r="L31" s="58" t="str">
-        <f>IFERROR(1-(M31/G31),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M31" s="57">
         <v>0</v>
       </c>
       <c r="N31" s="56">
-        <f>M31/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O31" s="55" t="str">
-        <f>IFERROR((K31-M31)/K31,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P31" s="54"/>
@@ -3589,25 +3583,25 @@
       <c r="H32" s="60"/>
       <c r="I32" s="59"/>
       <c r="J32" s="58" t="str">
-        <f>IFERROR(1-(K32/G32),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K32" s="57">
         <v>0</v>
       </c>
       <c r="L32" s="58" t="str">
-        <f>IFERROR(1-(M32/G32),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M32" s="57">
         <v>0</v>
       </c>
       <c r="N32" s="56">
-        <f>M32/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O32" s="55" t="str">
-        <f>IFERROR((K32-M32)/K32,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P32" s="54"/>
@@ -3624,25 +3618,25 @@
       <c r="H33" s="60"/>
       <c r="I33" s="59"/>
       <c r="J33" s="58" t="str">
-        <f>IFERROR(1-(K33/G33),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K33" s="57">
         <v>0</v>
       </c>
       <c r="L33" s="58" t="str">
-        <f>IFERROR(1-(M33/G33),"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="M33" s="57">
         <v>0</v>
       </c>
       <c r="N33" s="56">
-        <f>M33/0.9925</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O33" s="55" t="str">
-        <f>IFERROR((K33-M33)/K33,"")</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="P33" s="54"/>
@@ -3659,25 +3653,25 @@
       <c r="H34" s="60"/>
       <c r="I34" s="59"/>
       <c r="J34" s="58" t="str">
-        <f>IFERROR(1-(K34/G34),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K34" s="57">
         <v>0</v>
       </c>
       <c r="L34" s="58" t="str">
-        <f>IFERROR(1-(M34/G34),"")</f>
+        <f t="shared" ref="L34:L65" si="4">IFERROR(1-(M34/G34),"")</f>
         <v/>
       </c>
       <c r="M34" s="57">
         <v>0</v>
       </c>
       <c r="N34" s="56">
-        <f>M34/0.9925</f>
+        <f t="shared" ref="N34:N65" si="5">M34/0.9925</f>
         <v>0</v>
       </c>
       <c r="O34" s="55" t="str">
-        <f>IFERROR((K34-M34)/K34,"")</f>
+        <f t="shared" ref="O34:O58" si="6">IFERROR((K34-M34)/K34,"")</f>
         <v/>
       </c>
       <c r="P34" s="54"/>
@@ -3694,25 +3688,25 @@
       <c r="H35" s="60"/>
       <c r="I35" s="59"/>
       <c r="J35" s="58" t="str">
-        <f>IFERROR(1-(K35/G35),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K35" s="57">
         <v>0</v>
       </c>
       <c r="L35" s="58" t="str">
-        <f>IFERROR(1-(M35/G35),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M35" s="57">
         <v>0</v>
       </c>
       <c r="N35" s="56">
-        <f>M35/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O35" s="55" t="str">
-        <f>IFERROR((K35-M35)/K35,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P35" s="54"/>
@@ -3729,25 +3723,25 @@
       <c r="H36" s="60"/>
       <c r="I36" s="59"/>
       <c r="J36" s="58" t="str">
-        <f>IFERROR(1-(K36/G36),"")</f>
+        <f t="shared" ref="J36:J67" si="7">IFERROR(1-(K36/G36),"")</f>
         <v/>
       </c>
       <c r="K36" s="57">
         <v>0</v>
       </c>
       <c r="L36" s="58" t="str">
-        <f>IFERROR(1-(M36/G36),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M36" s="57">
         <v>0</v>
       </c>
       <c r="N36" s="56">
-        <f>M36/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O36" s="55" t="str">
-        <f>IFERROR((K36-M36)/K36,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P36" s="54"/>
@@ -3764,25 +3758,25 @@
       <c r="H37" s="60"/>
       <c r="I37" s="59"/>
       <c r="J37" s="58" t="str">
-        <f>IFERROR(1-(K37/G37),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K37" s="57">
         <v>0</v>
       </c>
       <c r="L37" s="58" t="str">
-        <f>IFERROR(1-(M37/G37),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M37" s="57">
         <v>0</v>
       </c>
       <c r="N37" s="56">
-        <f>M37/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O37" s="55" t="str">
-        <f>IFERROR((K37-M37)/K37,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P37" s="54"/>
@@ -3799,25 +3793,25 @@
       <c r="H38" s="60"/>
       <c r="I38" s="59"/>
       <c r="J38" s="58" t="str">
-        <f>IFERROR(1-(K38/G38),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K38" s="57">
         <v>0</v>
       </c>
       <c r="L38" s="58" t="str">
-        <f>IFERROR(1-(M38/G38),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M38" s="57">
         <v>0</v>
       </c>
       <c r="N38" s="56">
-        <f>M38/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O38" s="55" t="str">
-        <f>IFERROR((K38-M38)/K38,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P38" s="54"/>
@@ -3834,25 +3828,25 @@
       <c r="H39" s="60"/>
       <c r="I39" s="59"/>
       <c r="J39" s="58" t="str">
-        <f>IFERROR(1-(K39/G39),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K39" s="57">
         <v>0</v>
       </c>
       <c r="L39" s="58" t="str">
-        <f>IFERROR(1-(M39/G39),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M39" s="57">
         <v>0</v>
       </c>
       <c r="N39" s="56">
-        <f>M39/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O39" s="55" t="str">
-        <f>IFERROR((K39-M39)/K39,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P39" s="54"/>
@@ -3869,25 +3863,25 @@
       <c r="H40" s="60"/>
       <c r="I40" s="59"/>
       <c r="J40" s="58" t="str">
-        <f>IFERROR(1-(K40/G40),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K40" s="57">
         <v>0</v>
       </c>
       <c r="L40" s="58" t="str">
-        <f>IFERROR(1-(M40/G40),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M40" s="57">
         <v>0</v>
       </c>
       <c r="N40" s="56">
-        <f>M40/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O40" s="55" t="str">
-        <f>IFERROR((K40-M40)/K40,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P40" s="54"/>
@@ -3904,25 +3898,25 @@
       <c r="H41" s="60"/>
       <c r="I41" s="59"/>
       <c r="J41" s="58" t="str">
-        <f>IFERROR(1-(K41/G41),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K41" s="57">
         <v>0</v>
       </c>
       <c r="L41" s="58" t="str">
-        <f>IFERROR(1-(M41/G41),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M41" s="57">
         <v>0</v>
       </c>
       <c r="N41" s="56">
-        <f>M41/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O41" s="55" t="str">
-        <f>IFERROR((K41-M41)/K41,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P41" s="54"/>
@@ -3939,25 +3933,25 @@
       <c r="H42" s="60"/>
       <c r="I42" s="59"/>
       <c r="J42" s="58" t="str">
-        <f>IFERROR(1-(K42/G42),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K42" s="57">
         <v>0</v>
       </c>
       <c r="L42" s="58" t="str">
-        <f>IFERROR(1-(M42/G42),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M42" s="57">
         <v>0</v>
       </c>
       <c r="N42" s="56">
-        <f>M42/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O42" s="55" t="str">
-        <f>IFERROR((K42-M42)/K42,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P42" s="54"/>
@@ -3974,25 +3968,25 @@
       <c r="H43" s="60"/>
       <c r="I43" s="59"/>
       <c r="J43" s="58" t="str">
-        <f>IFERROR(1-(K43/G43),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K43" s="57">
         <v>0</v>
       </c>
       <c r="L43" s="58" t="str">
-        <f>IFERROR(1-(M43/G43),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M43" s="57">
         <v>0</v>
       </c>
       <c r="N43" s="56">
-        <f>M43/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O43" s="55" t="str">
-        <f>IFERROR((K43-M43)/K43,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P43" s="54"/>
@@ -4009,25 +4003,25 @@
       <c r="H44" s="60"/>
       <c r="I44" s="59"/>
       <c r="J44" s="58" t="str">
-        <f>IFERROR(1-(K44/G44),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K44" s="57">
         <v>0</v>
       </c>
       <c r="L44" s="58" t="str">
-        <f>IFERROR(1-(M44/G44),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M44" s="57">
         <v>0</v>
       </c>
       <c r="N44" s="56">
-        <f>M44/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O44" s="55" t="str">
-        <f>IFERROR((K44-M44)/K44,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P44" s="54"/>
@@ -4044,25 +4038,25 @@
       <c r="H45" s="60"/>
       <c r="I45" s="59"/>
       <c r="J45" s="58" t="str">
-        <f>IFERROR(1-(K45/G45),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K45" s="57">
         <v>0</v>
       </c>
       <c r="L45" s="58" t="str">
-        <f>IFERROR(1-(M45/G45),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M45" s="57">
         <v>0</v>
       </c>
       <c r="N45" s="56">
-        <f>M45/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O45" s="55" t="str">
-        <f>IFERROR((K45-M45)/K45,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P45" s="54"/>
@@ -4079,25 +4073,25 @@
       <c r="H46" s="60"/>
       <c r="I46" s="59"/>
       <c r="J46" s="58" t="str">
-        <f>IFERROR(1-(K46/G46),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K46" s="57">
         <v>0</v>
       </c>
       <c r="L46" s="58" t="str">
-        <f>IFERROR(1-(M46/G46),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M46" s="57">
         <v>0</v>
       </c>
       <c r="N46" s="56">
-        <f>M46/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O46" s="55" t="str">
-        <f>IFERROR((K46-M46)/K46,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P46" s="54"/>
@@ -4114,25 +4108,25 @@
       <c r="H47" s="60"/>
       <c r="I47" s="59"/>
       <c r="J47" s="58" t="str">
-        <f>IFERROR(1-(K47/G47),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K47" s="57">
         <v>0</v>
       </c>
       <c r="L47" s="58" t="str">
-        <f>IFERROR(1-(M47/G47),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M47" s="57">
         <v>0</v>
       </c>
       <c r="N47" s="56">
-        <f>M47/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O47" s="55" t="str">
-        <f>IFERROR((K47-M47)/K47,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P47" s="54"/>
@@ -4149,25 +4143,25 @@
       <c r="H48" s="60"/>
       <c r="I48" s="59"/>
       <c r="J48" s="58" t="str">
-        <f>IFERROR(1-(K48/G48),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K48" s="57">
         <v>0</v>
       </c>
       <c r="L48" s="58" t="str">
-        <f>IFERROR(1-(M48/G48),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M48" s="57">
         <v>0</v>
       </c>
       <c r="N48" s="56">
-        <f>M48/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O48" s="55" t="str">
-        <f>IFERROR((K48-M48)/K48,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P48" s="54"/>
@@ -4184,25 +4178,25 @@
       <c r="H49" s="60"/>
       <c r="I49" s="59"/>
       <c r="J49" s="58" t="str">
-        <f>IFERROR(1-(K49/G49),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K49" s="57">
         <v>0</v>
       </c>
       <c r="L49" s="58" t="str">
-        <f>IFERROR(1-(M49/G49),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M49" s="57">
         <v>0</v>
       </c>
       <c r="N49" s="56">
-        <f>M49/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O49" s="55" t="str">
-        <f>IFERROR((K49-M49)/K49,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P49" s="54"/>
@@ -4219,25 +4213,25 @@
       <c r="H50" s="60"/>
       <c r="I50" s="59"/>
       <c r="J50" s="58" t="str">
-        <f>IFERROR(1-(K50/G50),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K50" s="57">
         <v>0</v>
       </c>
       <c r="L50" s="58" t="str">
-        <f>IFERROR(1-(M50/G50),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M50" s="57">
         <v>0</v>
       </c>
       <c r="N50" s="56">
-        <f>M50/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O50" s="55" t="str">
-        <f>IFERROR((K50-M50)/K50,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P50" s="54"/>
@@ -4254,25 +4248,25 @@
       <c r="H51" s="60"/>
       <c r="I51" s="59"/>
       <c r="J51" s="58" t="str">
-        <f>IFERROR(1-(K51/G51),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K51" s="57">
         <v>0</v>
       </c>
       <c r="L51" s="58" t="str">
-        <f>IFERROR(1-(M51/G51),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M51" s="57">
         <v>0</v>
       </c>
       <c r="N51" s="56">
-        <f>M51/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O51" s="55" t="str">
-        <f>IFERROR((K51-M51)/K51,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P51" s="54"/>
@@ -4289,25 +4283,25 @@
       <c r="H52" s="60"/>
       <c r="I52" s="59"/>
       <c r="J52" s="58" t="str">
-        <f>IFERROR(1-(K52/G52),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K52" s="57">
         <v>0</v>
       </c>
       <c r="L52" s="58" t="str">
-        <f>IFERROR(1-(M52/G52),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M52" s="57">
         <v>0</v>
       </c>
       <c r="N52" s="56">
-        <f>M52/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O52" s="55" t="str">
-        <f>IFERROR((K52-M52)/K52,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P52" s="54"/>
@@ -4324,25 +4318,25 @@
       <c r="H53" s="60"/>
       <c r="I53" s="59"/>
       <c r="J53" s="58" t="str">
-        <f>IFERROR(1-(K53/G53),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K53" s="57">
         <v>0</v>
       </c>
       <c r="L53" s="58" t="str">
-        <f>IFERROR(1-(M53/G53),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M53" s="57">
         <v>0</v>
       </c>
       <c r="N53" s="56">
-        <f>M53/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O53" s="55" t="str">
-        <f>IFERROR((K53-M53)/K53,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P53" s="54"/>
@@ -4359,25 +4353,25 @@
       <c r="H54" s="60"/>
       <c r="I54" s="59"/>
       <c r="J54" s="58" t="str">
-        <f>IFERROR(1-(K54/G54),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K54" s="57">
         <v>0</v>
       </c>
       <c r="L54" s="58" t="str">
-        <f>IFERROR(1-(M54/G54),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M54" s="57">
         <v>0</v>
       </c>
       <c r="N54" s="56">
-        <f>M54/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O54" s="55" t="str">
-        <f>IFERROR((K54-M54)/K54,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P54" s="54"/>
@@ -4394,25 +4388,25 @@
       <c r="H55" s="60"/>
       <c r="I55" s="59"/>
       <c r="J55" s="58" t="str">
-        <f>IFERROR(1-(K55/G55),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K55" s="57">
         <v>0</v>
       </c>
       <c r="L55" s="58" t="str">
-        <f>IFERROR(1-(M55/G55),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M55" s="57">
         <v>0</v>
       </c>
       <c r="N55" s="56">
-        <f>M55/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O55" s="55" t="str">
-        <f>IFERROR((K55-M55)/K55,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P55" s="54"/>
@@ -4429,25 +4423,25 @@
       <c r="H56" s="60"/>
       <c r="I56" s="59"/>
       <c r="J56" s="58" t="str">
-        <f>IFERROR(1-(K56/G56),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K56" s="57">
         <v>0</v>
       </c>
       <c r="L56" s="58" t="str">
-        <f>IFERROR(1-(M56/G56),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M56" s="57">
         <v>0</v>
       </c>
       <c r="N56" s="56">
-        <f>M56/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O56" s="55" t="str">
-        <f>IFERROR((K56-M56)/K56,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P56" s="54"/>
@@ -4464,25 +4458,25 @@
       <c r="H57" s="60"/>
       <c r="I57" s="59"/>
       <c r="J57" s="58" t="str">
-        <f>IFERROR(1-(K57/G57),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K57" s="57">
         <v>0</v>
       </c>
       <c r="L57" s="58" t="str">
-        <f>IFERROR(1-(M57/G57),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M57" s="57">
         <v>0</v>
       </c>
       <c r="N57" s="56">
-        <f>M57/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O57" s="55" t="str">
-        <f>IFERROR((K57-M57)/K57,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P57" s="54"/>
@@ -4499,25 +4493,25 @@
       <c r="H58" s="60"/>
       <c r="I58" s="59"/>
       <c r="J58" s="58" t="str">
-        <f>IFERROR(1-(K58/G58),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="K58" s="57">
         <v>0</v>
       </c>
       <c r="L58" s="58" t="str">
-        <f>IFERROR(1-(M58/G58),"")</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="M58" s="57">
         <v>0</v>
       </c>
       <c r="N58" s="56">
-        <f>M58/0.9925</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="O58" s="55" t="str">
-        <f>IFERROR((K58-M58)/K58,"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="P58" s="54"/>
@@ -4525,7 +4519,7 @@
     </row>
   </sheetData>
   <sheetProtection formatColumns="0" formatRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0"/>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="16" type="noConversion"/>
   <dataValidations count="4">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D58">
       <formula1>0</formula1>

</xml_diff>